<commit_message>
charlem est en forme
</commit_message>
<xml_diff>
--- a/excel/week1.xlsx
+++ b/excel/week1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remilevesque/foot2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57FA0E2-F0E5-6647-94E5-E364A9694BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52015E5-636A-B74A-BC09-554A6534B7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="103">
   <si>
     <t>Timestamp</t>
   </si>
@@ -49,6 +49,48 @@
     <t>Chargers vs Jaguars Over Under (47.5)</t>
   </si>
   <si>
+    <t xml:space="preserve">Miami vs Bills </t>
+  </si>
+  <si>
+    <t>Miami vs Bills Score</t>
+  </si>
+  <si>
+    <t>Miami vs Bills Over Under (43.5)</t>
+  </si>
+  <si>
+    <t>Giants vs Vikings</t>
+  </si>
+  <si>
+    <t>Giants vs Vikings Score</t>
+  </si>
+  <si>
+    <t>Giants vs Vikings Over Under (48)</t>
+  </si>
+  <si>
+    <t>Ravens vs Bengals</t>
+  </si>
+  <si>
+    <t>Ravens vs Bengals Score</t>
+  </si>
+  <si>
+    <t>Ravens vs Bengals Over Under (40.5)</t>
+  </si>
+  <si>
+    <t>Cowboys vs Buccs</t>
+  </si>
+  <si>
+    <t>Cowboys vs Buccs Score</t>
+  </si>
+  <si>
+    <t>Cowboys vs Buccs Over Under (45.5)</t>
+  </si>
+  <si>
+    <t>Numéro d'assurance sociale</t>
+  </si>
+  <si>
+    <t>Superbowl winner (10 points)</t>
+  </si>
+  <si>
     <t>Papa Guini</t>
   </si>
   <si>
@@ -70,9 +112,39 @@
     <t>24-20</t>
   </si>
   <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38-10 </t>
+  </si>
+  <si>
     <t>over</t>
   </si>
   <si>
+    <t>Vikings</t>
+  </si>
+  <si>
+    <t>27-24</t>
+  </si>
+  <si>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>37-16</t>
+  </si>
+  <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>24-19</t>
+  </si>
+  <si>
+    <t>1837 1816 1828</t>
+  </si>
+  <si>
+    <t>Chiefs</t>
+  </si>
+  <si>
     <t>Toppest G (charlem)</t>
   </si>
   <si>
@@ -85,6 +157,18 @@
     <t>31-28</t>
   </si>
   <si>
+    <t>34-13</t>
+  </si>
+  <si>
+    <t>24-16</t>
+  </si>
+  <si>
+    <t>topg.com</t>
+  </si>
+  <si>
+    <t>49ers</t>
+  </si>
+  <si>
     <t>ChocoLatine</t>
   </si>
   <si>
@@ -97,6 +181,24 @@
     <t>31- 27 Chargers</t>
   </si>
   <si>
+    <t>24-7 Bills</t>
+  </si>
+  <si>
+    <t>24-21 Vikings</t>
+  </si>
+  <si>
+    <t>24-7</t>
+  </si>
+  <si>
+    <t>Buccs</t>
+  </si>
+  <si>
+    <t>21-10 Buccs</t>
+  </si>
+  <si>
+    <t>SB Champ = 49 niners</t>
+  </si>
+  <si>
     <t>romi trump</t>
   </si>
   <si>
@@ -106,6 +208,24 @@
     <t>27-20</t>
   </si>
   <si>
+    <t>26-20</t>
+  </si>
+  <si>
+    <t>23-17</t>
+  </si>
+  <si>
+    <t>30-23</t>
+  </si>
+  <si>
+    <t>23-21</t>
+  </si>
+  <si>
+    <t>454 390 313</t>
+  </si>
+  <si>
+    <t>Chargers</t>
+  </si>
+  <si>
     <t>Naruto</t>
   </si>
   <si>
@@ -118,6 +238,21 @@
     <t>24 a 27</t>
   </si>
   <si>
+    <t>35 a 7</t>
+  </si>
+  <si>
+    <t>Giants (beurk)</t>
+  </si>
+  <si>
+    <t>21 a 14</t>
+  </si>
+  <si>
+    <t>21 a 27</t>
+  </si>
+  <si>
+    <t>21 a 17</t>
+  </si>
+  <si>
     <t>Casper le gentil fantôme (Dave)</t>
   </si>
   <si>
@@ -127,6 +262,21 @@
     <t>24 à 21</t>
   </si>
   <si>
+    <t>30 à 17</t>
+  </si>
+  <si>
+    <t>24 à 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 -17 </t>
+  </si>
+  <si>
+    <t>28 à 24</t>
+  </si>
+  <si>
+    <t>Masterlappy</t>
+  </si>
+  <si>
     <t>Fredy</t>
   </si>
   <si>
@@ -139,16 +289,46 @@
     <t>28-20</t>
   </si>
   <si>
+    <t>24-14</t>
+  </si>
+  <si>
+    <t>25-20</t>
+  </si>
+  <si>
     <t>Noiro le black</t>
   </si>
   <si>
     <t>28-24</t>
   </si>
   <si>
+    <t>24-10</t>
+  </si>
+  <si>
+    <t>28-10</t>
+  </si>
+  <si>
+    <t>28-21</t>
+  </si>
+  <si>
     <t>Doudo</t>
   </si>
   <si>
     <t>21-17</t>
+  </si>
+  <si>
+    <t>38-17</t>
+  </si>
+  <si>
+    <t>17-14</t>
+  </si>
+  <si>
+    <t>38-10</t>
+  </si>
+  <si>
+    <t>24-21</t>
+  </si>
+  <si>
+    <t>Bleu</t>
   </si>
 </sst>
 </file>
@@ -426,9 +606,9 @@
   </sheetPr>
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="166" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -487,407 +667,686 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>44939.676858773149</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>44939.934279189816</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>44940.316606215274</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>44940.376684062503</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>44940.479377314812</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="W6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>44940.491280011571</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>44940.63775991898</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="W8" s="1"/>
+      <c r="T8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>44940.662635416666</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V9" s="4">
+        <v>4206969</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>44940.704032928239</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>